<commit_message>
minor changes for population analysis
</commit_message>
<xml_diff>
--- a/Mouse_workbooks/CH_150730_A.xlsx
+++ b/Mouse_workbooks/CH_150730_A.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\docubase\Mouse_workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlie\Documents\SourceTree_local\docubase\Mouse_workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
   <si>
     <t>Mouse ID</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>HS1 and HS2 were 78 uM apart, and in L2/3. HS2 is the most superficial. This HVA is likely area AL.</t>
+  </si>
+  <si>
+    <t>Concatenate_0010_to_0012</t>
+  </si>
+  <si>
+    <t>concatenation of _0010 to _0012</t>
   </si>
 </sst>
 </file>
@@ -964,6 +970,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -975,21 +996,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1425,7 +1431,7 @@
   <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12:I12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1693,13 +1699,27 @@
       <c r="I12" s="42"/>
     </row>
     <row r="13" spans="1:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="40"/>
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="5">
+        <v>4</v>
+      </c>
+      <c r="E13" s="36">
+        <v>34</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>58</v>
+      </c>
       <c r="H13" s="41"/>
       <c r="I13" s="42"/>
     </row>
@@ -2674,51 +2694,56 @@
     <row r="102" spans="1:9" ht="39" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="105">
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="A5:I5"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="G97:I97"/>
+    <mergeCell ref="G98:I98"/>
+    <mergeCell ref="G99:I99"/>
+    <mergeCell ref="G100:I100"/>
+    <mergeCell ref="G101:I101"/>
+    <mergeCell ref="G92:I92"/>
+    <mergeCell ref="G93:I93"/>
+    <mergeCell ref="G94:I94"/>
+    <mergeCell ref="G95:I95"/>
+    <mergeCell ref="G96:I96"/>
+    <mergeCell ref="G87:I87"/>
+    <mergeCell ref="G88:I88"/>
+    <mergeCell ref="G89:I89"/>
+    <mergeCell ref="G90:I90"/>
+    <mergeCell ref="G91:I91"/>
+    <mergeCell ref="G82:I82"/>
+    <mergeCell ref="G83:I83"/>
+    <mergeCell ref="G84:I84"/>
+    <mergeCell ref="G85:I85"/>
+    <mergeCell ref="G86:I86"/>
+    <mergeCell ref="G77:I77"/>
+    <mergeCell ref="G78:I78"/>
+    <mergeCell ref="G79:I79"/>
+    <mergeCell ref="G80:I80"/>
+    <mergeCell ref="G81:I81"/>
+    <mergeCell ref="G72:I72"/>
+    <mergeCell ref="G73:I73"/>
+    <mergeCell ref="G74:I74"/>
+    <mergeCell ref="G75:I75"/>
+    <mergeCell ref="G76:I76"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="G69:I69"/>
+    <mergeCell ref="G70:I70"/>
+    <mergeCell ref="G71:I71"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="G63:I63"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="G66:I66"/>
+    <mergeCell ref="G57:I57"/>
+    <mergeCell ref="G58:I58"/>
+    <mergeCell ref="G59:I59"/>
+    <mergeCell ref="G60:I60"/>
+    <mergeCell ref="G61:I61"/>
+    <mergeCell ref="G52:I52"/>
+    <mergeCell ref="G53:I53"/>
+    <mergeCell ref="G54:I54"/>
+    <mergeCell ref="G55:I55"/>
+    <mergeCell ref="G56:I56"/>
     <mergeCell ref="G47:I47"/>
     <mergeCell ref="G48:I48"/>
     <mergeCell ref="G49:I49"/>
@@ -2729,56 +2754,51 @@
     <mergeCell ref="G44:I44"/>
     <mergeCell ref="G45:I45"/>
     <mergeCell ref="G46:I46"/>
-    <mergeCell ref="G57:I57"/>
-    <mergeCell ref="G58:I58"/>
-    <mergeCell ref="G59:I59"/>
-    <mergeCell ref="G60:I60"/>
-    <mergeCell ref="G61:I61"/>
-    <mergeCell ref="G52:I52"/>
-    <mergeCell ref="G53:I53"/>
-    <mergeCell ref="G54:I54"/>
-    <mergeCell ref="G55:I55"/>
-    <mergeCell ref="G56:I56"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="G68:I68"/>
-    <mergeCell ref="G69:I69"/>
-    <mergeCell ref="G70:I70"/>
-    <mergeCell ref="G71:I71"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="G63:I63"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="G65:I65"/>
-    <mergeCell ref="G66:I66"/>
-    <mergeCell ref="G77:I77"/>
-    <mergeCell ref="G78:I78"/>
-    <mergeCell ref="G79:I79"/>
-    <mergeCell ref="G80:I80"/>
-    <mergeCell ref="G81:I81"/>
-    <mergeCell ref="G72:I72"/>
-    <mergeCell ref="G73:I73"/>
-    <mergeCell ref="G74:I74"/>
-    <mergeCell ref="G75:I75"/>
-    <mergeCell ref="G76:I76"/>
-    <mergeCell ref="G87:I87"/>
-    <mergeCell ref="G88:I88"/>
-    <mergeCell ref="G89:I89"/>
-    <mergeCell ref="G90:I90"/>
-    <mergeCell ref="G91:I91"/>
-    <mergeCell ref="G82:I82"/>
-    <mergeCell ref="G83:I83"/>
-    <mergeCell ref="G84:I84"/>
-    <mergeCell ref="G85:I85"/>
-    <mergeCell ref="G86:I86"/>
-    <mergeCell ref="G97:I97"/>
-    <mergeCell ref="G98:I98"/>
-    <mergeCell ref="G99:I99"/>
-    <mergeCell ref="G100:I100"/>
-    <mergeCell ref="G101:I101"/>
-    <mergeCell ref="G92:I92"/>
-    <mergeCell ref="G93:I93"/>
-    <mergeCell ref="G94:I94"/>
-    <mergeCell ref="G95:I95"/>
-    <mergeCell ref="G96:I96"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.47222222222222221" right="0.56944444444444442" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2938,7 +2958,7 @@
       <c r="A2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="84">
+      <c r="B2" s="76">
         <v>42215</v>
       </c>
       <c r="C2" s="66"/>
@@ -3000,12 +3020,12 @@
       <c r="A8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-      <c r="G8" s="81"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="78"/>
     </row>
     <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
@@ -3033,12 +3053,12 @@
       <c r="A11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="82"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="83"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="79"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="80"/>
     </row>
     <row r="12" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3057,12 +3077,12 @@
       <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="77"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="82"/>
     </row>
     <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
@@ -3090,32 +3110,32 @@
       <c r="A18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="78"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="79"/>
+      <c r="B18" s="83"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
+      <c r="G18" s="84"/>
     </row>
     <row r="19" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:7" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B5:G5"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>